<commit_message>
Working on free recall example
</commit_message>
<xml_diff>
--- a/free_recall_SHINY/Test Data RGN/Huff et al Key.xlsx
+++ b/free_recall_SHINY/Test Data RGN/Huff et al Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\lrd\free_recall_SHINY\Test Data RGN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1438B676-586A-4FAE-B896-4EA99DB496E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F75B59-3F38-4B71-A23A-09283C3E2694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11370" yWindow="2715" windowWidth="10155" windowHeight="9360" xr2:uid="{0C69F891-69EB-4909-88C8-1D79C299BE10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="3" xr2:uid="{0C69F891-69EB-4909-88C8-1D79C299BE10}"/>
   </bookViews>
   <sheets>
     <sheet name="Version A" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="251">
   <si>
     <t>NUTMEG</t>
   </si>
@@ -788,9 +788,6 @@
   </si>
   <si>
     <t>JAR</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Cat_Recall_L6</t>
@@ -1147,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC29764-7A87-425E-93DB-BB69BC9DA1AC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2444,10 +2441,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F7C19F-B2C2-4317-BAF7-05920E979132}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2870,121 +2867,6 @@
       </c>
       <c r="F21" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3019,7 +2901,7 @@
         <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>